<commit_message>
Published state of ETDataset on September 27 2021
</commit_message>
<xml_diff>
--- a/analyses/12_molecules_analysis.xlsx
+++ b/analyses/12_molecules_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Code/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783DC9FC-B0F6-A047-9B0D-E9021A5B80EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781A43FF-AA21-7447-A08D-8A30957DB5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27820" windowHeight="17540" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -31,6 +31,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
     <definedName name="base_year">Dashboard!$E$12</definedName>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="124">
   <si>
     <t>Changelog</t>
   </si>
@@ -417,9 +418,6 @@
   </si>
   <si>
     <t>industry_steel_electricfurnace_capture_potential_co2_parent_share</t>
-  </si>
-  <si>
-    <t>nl</t>
   </si>
   <si>
     <t>Paper</t>
@@ -498,7 +496,7 @@
     <numFmt numFmtId="166" formatCode="0.00000000E+00"/>
     <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6643,6 +6641,28 @@
     <sheetNames>
       <sheetName val="Cover sheet"/>
       <sheetName val="Dashboard"/>
+      <sheetName val="analysis_manager"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="export_data_button"/>
+      <definedName name="import_data_button"/>
+      <definedName name="select_dashboard_values"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover sheet"/>
+      <sheetName val="Dashboard"/>
     </sheetNames>
     <definedNames>
       <definedName name="export_data_button"/>
@@ -6988,7 +7008,7 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
@@ -6997,22 +7017,22 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="21">
+    <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="str">
         <f>"Molecules analysis "&amp;C6&amp;" "&amp;C7</f>
-        <v>Molecules analysis nl 2015</v>
+        <v>Molecules analysis 0 0</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -7022,27 +7042,27 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="64" t="str">
+      <c r="C6" s="64">
         <f>Dashboard!E11</f>
-        <v>nl</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="63" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="65">
         <f>Dashboard!E12</f>
-        <v>2015</v>
+        <v>0</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
@@ -7052,7 +7072,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
@@ -7061,7 +7081,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>19</v>
       </c>
@@ -7070,19 +7090,19 @@
       </c>
       <c r="D10" s="11"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="21" t="s">
         <v>10</v>
       </c>
@@ -7091,33 +7111,33 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="2:4" ht="17" thickBot="1">
+    <row r="15" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="2:4" ht="17" thickBot="1">
+    <row r="16" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="21"/>
       <c r="C17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="21"/>
       <c r="C18" s="8"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
         <v>57</v>
       </c>
@@ -7126,113 +7146,113 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="21"/>
       <c r="C20" s="57" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="21"/>
       <c r="C21" s="58" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="21"/>
       <c r="C22" s="59" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="19"/>
       <c r="C23" s="25" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="19"/>
       <c r="C24" s="60" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="19"/>
       <c r="C25" s="61" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="19"/>
       <c r="C26" s="50" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="20"/>
       <c r="C27" s="120"/>
       <c r="D27" s="11"/>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="19"/>
       <c r="C30" s="121"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="19"/>
       <c r="C31" s="8"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="19"/>
       <c r="C32" s="8"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="19"/>
       <c r="C33" s="8"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="19"/>
       <c r="C34" s="8"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="19"/>
       <c r="C35" s="8"/>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="19"/>
       <c r="C36" s="8"/>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="19"/>
       <c r="C37" s="8"/>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="19"/>
       <c r="C38" s="8"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="20"/>
       <c r="C39" s="10"/>
       <c r="D39" s="11"/>
@@ -7258,18 +7278,18 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7277,7 +7297,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -7286,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -7311,18 +7331,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7330,7 +7350,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -7339,7 +7359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -7364,18 +7384,18 @@
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7383,18 +7403,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E40</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E41</f>
@@ -7417,18 +7437,18 @@
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7436,18 +7456,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E43</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E44</f>
@@ -7470,18 +7490,18 @@
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7489,18 +7509,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E48</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E49</f>
@@ -7523,18 +7543,18 @@
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7542,18 +7562,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E51</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E52</f>
@@ -7576,7 +7596,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -7585,12 +7605,12 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="21">
+    <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
@@ -7601,12 +7621,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="91">
         <v>44078</v>
       </c>
@@ -7617,18 +7637,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="17">
+    <row r="7" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="91">
         <v>44084</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="18">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="20"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
@@ -7650,7 +7670,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="56.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -7658,12 +7678,12 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="48" t="s">
         <v>21</v>
       </c>
@@ -7671,11 +7691,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="36"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="2:3" ht="28" customHeight="1">
+    <row r="6" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="122" t="s">
         <v>41</v>
       </c>
@@ -7683,7 +7703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="28" customHeight="1">
+    <row r="7" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="122" t="s">
         <v>0</v>
       </c>
@@ -7691,7 +7711,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="28" customHeight="1">
+    <row r="8" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="122" t="s">
         <v>20</v>
       </c>
@@ -7699,7 +7719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="28" customHeight="1">
+    <row r="9" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="122" t="s">
         <v>24</v>
       </c>
@@ -7707,7 +7727,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="28" customHeight="1">
+    <row r="10" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="125" t="s">
         <v>26</v>
       </c>
@@ -7715,7 +7735,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="28" customHeight="1">
+    <row r="11" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="126" t="s">
         <v>74</v>
       </c>
@@ -7723,7 +7743,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="28" customHeight="1"/>
+    <row r="12" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7741,82 +7761,82 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="143.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="21">
+    <row r="2" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" s="40"/>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="138"/>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" s="51"/>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" s="52" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" s="53"/>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" s="139" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" s="139" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B12" s="139" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" s="139" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" s="139" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" s="139" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" s="39"/>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="48" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="40"/>
     </row>
-    <row r="20" spans="2:2" ht="102">
+    <row r="20" spans="2:2" ht="102" x14ac:dyDescent="0.2">
       <c r="B20" s="49" t="s">
         <v>70</v>
       </c>
@@ -7834,11 +7854,11 @@
   </sheetPr>
   <dimension ref="B2:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="17.1640625" style="44" customWidth="1"/>
@@ -7859,7 +7879,7 @@
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="21">
+    <row r="2" spans="2:16" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
@@ -7870,14 +7890,14 @@
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="81"/>
       <c r="I3" s="112"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="33" t="s">
         <v>33</v>
       </c>
@@ -7890,7 +7910,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="2:16" ht="45" customHeight="1">
+    <row r="5" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="154" t="s">
         <v>49</v>
       </c>
@@ -7903,8 +7923,8 @@
       <c r="K5" s="10"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="2:16" ht="17" thickBot="1"/>
-    <row r="7" spans="2:16">
+    <row r="6" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="s">
         <v>25</v>
       </c>
@@ -7925,7 +7945,7 @@
       <c r="O7" s="116"/>
       <c r="P7" s="117"/>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="45"/>
       <c r="C8" s="68"/>
       <c r="D8" s="76"/>
@@ -7942,7 +7962,7 @@
       <c r="O8" s="113"/>
       <c r="P8" s="115"/>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="127" t="s">
         <v>35</v>
       </c>
@@ -7981,7 +8001,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="129" t="s">
         <v>32</v>
       </c>
@@ -8005,15 +8025,13 @@
       <c r="O10" s="113"/>
       <c r="P10" s="115"/>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="31"/>
       <c r="C11" s="43" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="106"/>
-      <c r="E11" s="43" t="s">
-        <v>102</v>
-      </c>
+      <c r="E11" s="43"/>
       <c r="F11" s="68"/>
       <c r="G11" s="22" t="s">
         <v>67</v>
@@ -8030,15 +8048,13 @@
       </c>
       <c r="P11" s="115"/>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="31"/>
       <c r="C12" s="43" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="106"/>
-      <c r="E12" s="43">
-        <v>2015</v>
-      </c>
+      <c r="E12" s="43"/>
       <c r="F12" s="68"/>
       <c r="G12" s="22" t="s">
         <v>66</v>
@@ -8050,7 +8066,7 @@
         <v>45</v>
       </c>
       <c r="L12" s="133" t="b">
-        <f>IF(COUNTBLANK(E11:E54)-COUNTBLANK(C11:C54)=3,TRUE,FALSE)</f>
+        <f>IF(COUNTBLANK(E11:E54)-COUNTBLANK(C11:C54)=4,TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="M12" s="87"/>
@@ -8063,7 +8079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="31"/>
       <c r="C13" s="15"/>
       <c r="D13" s="77"/>
@@ -8080,7 +8096,7 @@
       <c r="O13" s="113"/>
       <c r="P13" s="115"/>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="31"/>
       <c r="C14" s="15"/>
       <c r="D14" s="77"/>
@@ -8097,10 +8113,10 @@
       <c r="O14" s="113"/>
       <c r="P14" s="115"/>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="30"/>
       <c r="C15" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D15" s="78"/>
       <c r="E15" s="79"/>
@@ -8116,7 +8132,7 @@
       <c r="O15" s="113"/>
       <c r="P15" s="115"/>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
         <v>81</v>
       </c>
@@ -8135,7 +8151,7 @@
       <c r="O16" s="113"/>
       <c r="P16" s="115"/>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="32"/>
       <c r="C17" s="15"/>
       <c r="D17" s="77"/>
@@ -8152,7 +8168,7 @@
       <c r="O17" s="113"/>
       <c r="P17" s="115"/>
     </row>
-    <row r="18" spans="2:16" ht="18" thickBot="1">
+    <row r="18" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="135" t="s">
         <v>85</v>
@@ -8179,7 +8195,7 @@
       <c r="O18" s="113"/>
       <c r="P18" s="115"/>
     </row>
-    <row r="19" spans="2:16" ht="17" thickBot="1">
+    <row r="19" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="134" t="s">
         <v>75</v>
@@ -8205,7 +8221,7 @@
       </c>
       <c r="P19" s="115"/>
     </row>
-    <row r="20" spans="2:16" ht="17" thickBot="1">
+    <row r="20" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="134" t="s">
         <v>76</v>
@@ -8231,7 +8247,7 @@
       </c>
       <c r="P20" s="115"/>
     </row>
-    <row r="21" spans="2:16" ht="17" thickBot="1">
+    <row r="21" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="134"/>
       <c r="D21" s="148"/>
@@ -8251,7 +8267,7 @@
       <c r="O21" s="113"/>
       <c r="P21" s="115"/>
     </row>
-    <row r="22" spans="2:16" ht="17" thickBot="1">
+    <row r="22" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="134" t="s">
         <v>84</v>
@@ -8273,7 +8289,7 @@
       </c>
       <c r="P22" s="115"/>
     </row>
-    <row r="23" spans="2:16" ht="17" thickBot="1">
+    <row r="23" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
       <c r="C23" s="134" t="s">
         <v>76</v>
@@ -8299,7 +8315,7 @@
       </c>
       <c r="P23" s="115"/>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="32"/>
       <c r="C24" s="15"/>
       <c r="D24" s="77"/>
@@ -8316,7 +8332,7 @@
       <c r="O24" s="113"/>
       <c r="P24" s="115"/>
     </row>
-    <row r="25" spans="2:16" ht="18" thickBot="1">
+    <row r="25" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
       <c r="C25" s="135" t="s">
         <v>82</v>
@@ -8343,7 +8359,7 @@
       <c r="O25" s="113"/>
       <c r="P25" s="115"/>
     </row>
-    <row r="26" spans="2:16" ht="17" thickBot="1">
+    <row r="26" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26" s="134" t="s">
         <v>75</v>
@@ -8369,7 +8385,7 @@
       </c>
       <c r="P26" s="115"/>
     </row>
-    <row r="27" spans="2:16" ht="17" thickBot="1">
+    <row r="27" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
       <c r="C27" s="134" t="s">
         <v>76</v>
@@ -8395,7 +8411,7 @@
       </c>
       <c r="P27" s="115"/>
     </row>
-    <row r="28" spans="2:16" ht="17" thickBot="1">
+    <row r="28" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
       <c r="C28" s="134"/>
       <c r="D28" s="106"/>
@@ -8415,7 +8431,7 @@
       <c r="O28" s="113"/>
       <c r="P28" s="115"/>
     </row>
-    <row r="29" spans="2:16" ht="17" thickBot="1">
+    <row r="29" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
       <c r="C29" s="134" t="s">
         <v>84</v>
@@ -8437,7 +8453,7 @@
       </c>
       <c r="P29" s="115"/>
     </row>
-    <row r="30" spans="2:16" ht="17" thickBot="1">
+    <row r="30" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
       <c r="C30" s="134" t="s">
         <v>76</v>
@@ -8463,7 +8479,7 @@
       </c>
       <c r="P30" s="115"/>
     </row>
-    <row r="31" spans="2:16">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="32"/>
       <c r="C31" s="134"/>
       <c r="D31" s="106"/>
@@ -8480,7 +8496,7 @@
       <c r="O31" s="113"/>
       <c r="P31" s="115"/>
     </row>
-    <row r="32" spans="2:16" ht="18" thickBot="1">
+    <row r="32" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
       <c r="C32" s="135" t="s">
         <v>95</v>
@@ -8507,7 +8523,7 @@
       <c r="O32" s="113"/>
       <c r="P32" s="115"/>
     </row>
-    <row r="33" spans="2:16" ht="17" thickBot="1">
+    <row r="33" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
       <c r="C33" s="134" t="s">
         <v>75</v>
@@ -8533,7 +8549,7 @@
       </c>
       <c r="P33" s="115"/>
     </row>
-    <row r="34" spans="2:16" ht="17" thickBot="1">
+    <row r="34" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
       <c r="C34" s="134" t="s">
         <v>76</v>
@@ -8559,7 +8575,7 @@
       </c>
       <c r="P34" s="115"/>
     </row>
-    <row r="35" spans="2:16" ht="17" thickBot="1">
+    <row r="35" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="32"/>
       <c r="C35" s="134"/>
       <c r="D35" s="106"/>
@@ -8579,7 +8595,7 @@
       <c r="O35" s="113"/>
       <c r="P35" s="115"/>
     </row>
-    <row r="36" spans="2:16" ht="17" thickBot="1">
+    <row r="36" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
       <c r="C36" s="134" t="s">
         <v>84</v>
@@ -8601,7 +8617,7 @@
       </c>
       <c r="P36" s="115"/>
     </row>
-    <row r="37" spans="2:16" ht="17" thickBot="1">
+    <row r="37" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
       <c r="C37" s="134" t="s">
         <v>76</v>
@@ -8627,7 +8643,7 @@
       </c>
       <c r="P37" s="115"/>
     </row>
-    <row r="38" spans="2:16">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="32"/>
       <c r="C38" s="134"/>
       <c r="D38" s="106"/>
@@ -8644,9 +8660,9 @@
       <c r="O38" s="113"/>
       <c r="P38" s="115"/>
     </row>
-    <row r="39" spans="2:16" ht="17" thickBot="1">
+    <row r="39" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39" s="134"/>
       <c r="D39" s="106"/>
@@ -8666,7 +8682,7 @@
       <c r="O39" s="113"/>
       <c r="P39" s="115"/>
     </row>
-    <row r="40" spans="2:16" ht="17" thickBot="1">
+    <row r="40" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
       <c r="C40" s="134" t="s">
         <v>75</v>
@@ -8688,11 +8704,11 @@
       </c>
       <c r="N40" s="46"/>
       <c r="O40" s="113" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P40" s="115"/>
     </row>
-    <row r="41" spans="2:16" ht="17" thickBot="1">
+    <row r="41" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
       <c r="C41" s="134" t="s">
         <v>76</v>
@@ -8714,11 +8730,11 @@
       <c r="M41" s="88"/>
       <c r="N41" s="46"/>
       <c r="O41" s="113" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P41" s="115"/>
     </row>
-    <row r="42" spans="2:16" ht="17" thickBot="1">
+    <row r="42" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
       <c r="C42" s="134"/>
       <c r="D42" s="148"/>
@@ -8738,7 +8754,7 @@
       <c r="O42" s="113"/>
       <c r="P42" s="115"/>
     </row>
-    <row r="43" spans="2:16" ht="17" thickBot="1">
+    <row r="43" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
       <c r="C43" s="134" t="s">
         <v>84</v>
@@ -8756,11 +8772,11 @@
       <c r="M43" s="88"/>
       <c r="N43" s="46"/>
       <c r="O43" s="113" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P43" s="115"/>
     </row>
-    <row r="44" spans="2:16" ht="17" thickBot="1">
+    <row r="44" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
       <c r="C44" s="134" t="s">
         <v>76</v>
@@ -8782,11 +8798,11 @@
       <c r="M44" s="88"/>
       <c r="N44" s="46"/>
       <c r="O44" s="113" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P44" s="115"/>
     </row>
-    <row r="45" spans="2:16">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B45" s="32"/>
       <c r="C45" s="134"/>
       <c r="D45" s="106"/>
@@ -8803,7 +8819,7 @@
       <c r="O45" s="113"/>
       <c r="P45" s="115"/>
     </row>
-    <row r="46" spans="2:16">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B46" s="32"/>
       <c r="C46" s="134"/>
       <c r="D46" s="106"/>
@@ -8820,9 +8836,9 @@
       <c r="O46" s="113"/>
       <c r="P46" s="115"/>
     </row>
-    <row r="47" spans="2:16" ht="17" thickBot="1">
+    <row r="47" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C47" s="134"/>
       <c r="D47" s="106"/>
@@ -8842,7 +8858,7 @@
       <c r="O47" s="113"/>
       <c r="P47" s="115"/>
     </row>
-    <row r="48" spans="2:16" ht="17" thickBot="1">
+    <row r="48" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
       <c r="C48" s="134" t="s">
         <v>75</v>
@@ -8864,11 +8880,11 @@
       </c>
       <c r="N48" s="46"/>
       <c r="O48" s="113" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P48" s="115"/>
     </row>
-    <row r="49" spans="2:16" ht="17" thickBot="1">
+    <row r="49" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="32"/>
       <c r="C49" s="134" t="s">
         <v>76</v>
@@ -8890,11 +8906,11 @@
       <c r="M49" s="88"/>
       <c r="N49" s="46"/>
       <c r="O49" s="113" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P49" s="115"/>
     </row>
-    <row r="50" spans="2:16" ht="17" thickBot="1">
+    <row r="50" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="32"/>
       <c r="C50" s="134"/>
       <c r="D50" s="148"/>
@@ -8914,7 +8930,7 @@
       <c r="O50" s="113"/>
       <c r="P50" s="115"/>
     </row>
-    <row r="51" spans="2:16" ht="17" thickBot="1">
+    <row r="51" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="32"/>
       <c r="C51" s="134" t="s">
         <v>84</v>
@@ -8932,11 +8948,11 @@
       <c r="M51" s="88"/>
       <c r="N51" s="46"/>
       <c r="O51" s="113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P51" s="115"/>
     </row>
-    <row r="52" spans="2:16" ht="17" thickBot="1">
+    <row r="52" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="32"/>
       <c r="C52" s="134" t="s">
         <v>76</v>
@@ -8958,11 +8974,11 @@
       <c r="M52" s="88"/>
       <c r="N52" s="46"/>
       <c r="O52" s="113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P52" s="115"/>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="32"/>
       <c r="C53" s="134"/>
       <c r="D53" s="106"/>
@@ -8979,7 +8995,7 @@
       <c r="O53" s="113"/>
       <c r="P53" s="115"/>
     </row>
-    <row r="54" spans="2:16" ht="17" thickBot="1">
+    <row r="54" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="109"/>
       <c r="C54" s="70"/>
       <c r="D54" s="143"/>
@@ -8996,63 +9012,63 @@
       <c r="O54" s="146"/>
       <c r="P54" s="147"/>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G55" s="102"/>
       <c r="H55" s="96"/>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G56" s="102"/>
       <c r="H56" s="96"/>
     </row>
-    <row r="57" spans="2:16">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G57" s="104"/>
     </row>
-    <row r="58" spans="2:16">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G58" s="104"/>
     </row>
-    <row r="59" spans="2:16">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G59" s="105"/>
       <c r="H59" s="66"/>
       <c r="I59" s="66"/>
       <c r="J59" s="66"/>
       <c r="K59" s="66"/>
     </row>
-    <row r="60" spans="2:16">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G60" s="105"/>
       <c r="H60" s="66"/>
       <c r="I60" s="66"/>
       <c r="J60" s="66"/>
       <c r="K60" s="66"/>
     </row>
-    <row r="61" spans="2:16">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G61" s="105"/>
       <c r="H61" s="66"/>
       <c r="I61" s="66"/>
       <c r="J61" s="66"/>
       <c r="K61" s="66"/>
     </row>
-    <row r="62" spans="2:16">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G62" s="105"/>
       <c r="H62" s="66"/>
       <c r="I62" s="66"/>
       <c r="J62" s="66"/>
       <c r="K62" s="66"/>
     </row>
-    <row r="63" spans="2:16">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G63" s="105"/>
       <c r="H63" s="66"/>
       <c r="I63" s="66"/>
       <c r="J63" s="66"/>
       <c r="K63" s="66"/>
     </row>
-    <row r="64" spans="2:16">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G64" s="105"/>
       <c r="H64" s="66"/>
       <c r="I64" s="66"/>
       <c r="J64" s="66"/>
       <c r="K64" s="66"/>
     </row>
-    <row r="65" spans="7:11">
+    <row r="65" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G65" s="105"/>
       <c r="H65" s="66"/>
       <c r="I65" s="66"/>
@@ -9138,7 +9154,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3073" r:id="rId3" name="import_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!import_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!import_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -9160,7 +9176,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3074" r:id="rId4" name="export_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!export_data_button" altText="export to 'data/…/ouput/molecules’ folder">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!export_data_button" altText="export to 'data/…/ouput/molecules’ folder">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -9182,7 +9198,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3076" r:id="rId5" name="select_dashboard">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!select_dashboard_values">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!select_dashboard_values">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -9218,18 +9234,18 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9237,7 +9253,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -9246,7 +9262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -9271,18 +9287,18 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9290,7 +9306,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -9299,7 +9315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -9324,18 +9340,18 @@
       <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9343,7 +9359,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -9352,7 +9368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -9377,18 +9393,18 @@
       <selection activeCell="B5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9396,7 +9412,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -9405,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Publish state of ETDataset on 20 December 2021
</commit_message>
<xml_diff>
--- a/analyses/12_molecules_analysis.xlsx
+++ b/analyses/12_molecules_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Code/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lottevanvlimmeren/Code/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781A43FF-AA21-7447-A08D-8A30957DB5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836BCB40-FBBE-4E46-8077-2D5345B264CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="932" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Contents" sheetId="18" r:id="rId3"/>
     <sheet name="Introduction" sheetId="10" r:id="rId4"/>
     <sheet name="Dashboard" sheetId="28" r:id="rId5"/>
-    <sheet name="csv_mol_steel_blast_pot_ps" sheetId="116" r:id="rId6"/>
+    <sheet name="csv_mol_steel_blast_bof_pot_ps" sheetId="116" r:id="rId6"/>
     <sheet name="csv_mol_steel_blast_current_ps" sheetId="115" r:id="rId7"/>
-    <sheet name="csv_mol_steel_hisarna_pot_ps" sheetId="113" r:id="rId8"/>
-    <sheet name="csv_mol_steel_hisarna_curr_ps" sheetId="114" r:id="rId9"/>
-    <sheet name="csv_mol_steel_elecfur_pot_ps" sheetId="117" r:id="rId10"/>
-    <sheet name="csv_mol_steel_elecfur_curr_ps" sheetId="118" r:id="rId11"/>
+    <sheet name="csv_mol_steel_cyclone_pot_ps" sheetId="113" r:id="rId8"/>
+    <sheet name="csv_mol_steel_cyclone_curr_ps" sheetId="114" r:id="rId9"/>
+    <sheet name="csv_mol_steel_dri_eaf_pot_ps" sheetId="117" r:id="rId10"/>
+    <sheet name="csv_mol_steel_dri_eaf_curr_ps" sheetId="118" r:id="rId11"/>
     <sheet name="csv_mol_paper_potential_ps" sheetId="119" r:id="rId12"/>
     <sheet name="csv_mol_paper_current_ps" sheetId="120" r:id="rId13"/>
     <sheet name="csv_mol_food_potential_ps" sheetId="123" r:id="rId14"/>
@@ -31,7 +31,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId16"/>
-    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
     <definedName name="base_year">Dashboard!$E$12</definedName>
@@ -112,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="129">
   <si>
     <t>Changelog</t>
   </si>
@@ -333,9 +332,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Roos de Kok</t>
-  </si>
-  <si>
     <t>csv_fertilizers</t>
   </si>
   <si>
@@ -348,78 +344,15 @@
     <t>%</t>
   </si>
   <si>
-    <t>industry_steel_hisarna_co2_parent_share</t>
-  </si>
-  <si>
-    <t>industry_steel_hisarna_capture_potential_co2</t>
-  </si>
-  <si>
     <t>industry_steel_emitted_co2</t>
   </si>
   <si>
     <t>Steel</t>
   </si>
   <si>
-    <t>Hisarna</t>
-  </si>
-  <si>
-    <t>industry_steel_hisarna_emitted_co2</t>
-  </si>
-  <si>
     <t>Share of potential currently used</t>
   </si>
   <si>
-    <t>Blastfurnace</t>
-  </si>
-  <si>
-    <t>industry_steel_hisarna_captured_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_hisarna_capture_potential_emitted_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_hisarna_capture_potential_co2_parent_share</t>
-  </si>
-  <si>
-    <t>industry_steel_blastfurnace_capture_potential_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_blastfurnace_emitted_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_blastfurnace_captured_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_blastfurnace_potential_emitted_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_blastfurnace_co2_parent_share</t>
-  </si>
-  <si>
-    <t>industry_steel_blastfurnace_capture_potential_co2_parent_share</t>
-  </si>
-  <si>
-    <t>Electric furnace</t>
-  </si>
-  <si>
-    <t>industry_steel_electricfurnace_capture_potential_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_electricfurnace_emitted_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_electricfurnace_captured_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_electricfurnace_capture_potential_emitted_co2</t>
-  </si>
-  <si>
-    <t>industry_steel_electricfurnace_co2_parent_share</t>
-  </si>
-  <si>
-    <t>industry_steel_electricfurnace_capture_potential_co2_parent_share</t>
-  </si>
-  <si>
     <t>Paper</t>
   </si>
   <si>
@@ -450,40 +383,121 @@
     <t>industry_food_potential_emitted_co2</t>
   </si>
   <si>
+    <t>industry_other_paper_capture_potential_co2</t>
+  </si>
+  <si>
+    <t>industry_other_paper_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_other_paper_captured_co2</t>
+  </si>
+  <si>
+    <t>industry_other_food_capture_potential_co2</t>
+  </si>
+  <si>
+    <t>industry_other_food_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_other_food_captured_co2</t>
+  </si>
+  <si>
+    <t>Note: Fertilizers is part of the Chemical industry analysis (4b).</t>
+  </si>
+  <si>
+    <t>Add steel, paper, food</t>
+  </si>
+  <si>
+    <t>Blastfurnace BOF</t>
+  </si>
+  <si>
+    <t>Cyclonefurnace BOF</t>
+  </si>
+  <si>
+    <t>industry_steel_blastfurnace_bof_capture_potential_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_blastfurnace_bof_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_blastfurnace_bof_captured_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_blastfurnace_bofpotential_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_cyclonefurnace_bof_capture_potential_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_cyclonefurnace_bof_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_cyclonefurnace_bof_captured_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_cyclonefurnace_bof_capture_potential_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_eaf_capture_potential_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_eaf_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_eaf_captured_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_eaf_capture_potential_emitted_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_blastfurnace_bof_co2_parent_share</t>
+  </si>
+  <si>
+    <t>industry_steel_blastfurnace_bof_capture_potential_co2_parent_share</t>
+  </si>
+  <si>
+    <t>industry_steel_cyclonefurnace_bof_co2_parent_share</t>
+  </si>
+  <si>
+    <t>industry_steel_cyclonefurnace_bof_capture_potential_co2_parent_share</t>
+  </si>
+  <si>
+    <t>Adjusted the steel production technologies during the steel update: renamed blastfurnace to blastfurnace BOF, renamed Hisarna to Cyclonefurnace BOF, removed Electric Arc Furnace, added DRI network gas EAF and DRI network gas EAF + BOF.</t>
+  </si>
+  <si>
+    <t>November 26, 2021</t>
+  </si>
+  <si>
+    <t>Lotte van Vlimmeren</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>industry_other_paper_capture_potential_co2_parent_share</t>
+  </si>
+  <si>
     <t>industry_other_paper_combustion_co2_parent_share</t>
   </si>
   <si>
-    <t>industry_other_paper_capture_potential_co2</t>
-  </si>
-  <si>
-    <t>industry_other_paper_emitted_co2</t>
-  </si>
-  <si>
-    <t>industry_other_paper_capture_potential_co2_parent_share</t>
-  </si>
-  <si>
-    <t>industry_other_paper_captured_co2</t>
+    <t>industry_other_food_capture_potential_co2_parent_share</t>
   </si>
   <si>
     <t>industry_other_food_combustion_co2_parent_share</t>
   </si>
   <si>
-    <t>industry_other_food_capture_potential_co2</t>
-  </si>
-  <si>
-    <t>industry_other_food_emitted_co2</t>
-  </si>
-  <si>
-    <t>industry_other_food_capture_potential_co2_parent_share</t>
-  </si>
-  <si>
-    <t>industry_other_food_captured_co2</t>
-  </si>
-  <si>
-    <t>Note: Fertilizers is part of the Chemical industry analysis (4b).</t>
-  </si>
-  <si>
-    <t>Add steel, paper, food</t>
+    <t>DRI network gas</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_co2_parent_share</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_capture_potential_co2</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_capture_potential_co2_parent_share</t>
+  </si>
+  <si>
+    <t>industry_steel_dri_network_gas_captured_co2</t>
   </si>
 </sst>
 </file>
@@ -6641,28 +6655,6 @@
     <sheetNames>
       <sheetName val="Cover sheet"/>
       <sheetName val="Dashboard"/>
-      <sheetName val="analysis_manager"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="export_data_button"/>
-      <definedName name="import_data_button"/>
-      <definedName name="select_dashboard_values"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover sheet"/>
-      <sheetName val="Dashboard"/>
     </sheetNames>
     <definedNames>
       <definedName name="export_data_button"/>
@@ -7005,7 +6997,7 @@
   <dimension ref="B2:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7028,7 +7020,7 @@
       </c>
       <c r="C4" s="4" t="str">
         <f>"Molecules analysis "&amp;C6&amp;" "&amp;C7</f>
-        <v>Molecules analysis 0 0</v>
+        <v>Molecules analysis nl 2019</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -7038,7 +7030,7 @@
       </c>
       <c r="C5" s="110">
         <f>MAX(Changelog!D:D)</f>
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -7046,9 +7038,9 @@
       <c r="B6" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="64" t="str">
         <f>Dashboard!E11</f>
-        <v>0</v>
+        <v>nl</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -7058,7 +7050,7 @@
       </c>
       <c r="C7" s="65">
         <f>Dashboard!E12</f>
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -7066,9 +7058,8 @@
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="92">
-        <f>MAX(Changelog!B:B)</f>
-        <v>44084</v>
+      <c r="C8" s="92" t="s">
+        <v>117</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -7077,7 +7068,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -7262,7 +7253,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="C5 C8" emptyCellReference="1"/>
+    <ignoredError sqref="C5" emptyCellReference="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -7275,7 +7266,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7286,7 +7277,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7299,7 +7290,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E33</f>
@@ -7308,7 +7299,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E34</f>
@@ -7327,8 +7318,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7339,7 +7330,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7352,7 +7343,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E22</f>
@@ -7361,7 +7352,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E23</f>
@@ -7381,7 +7372,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7392,7 +7383,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7405,7 +7396,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E40</f>
@@ -7414,7 +7405,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E41</f>
@@ -7434,7 +7425,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7445,7 +7436,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7458,7 +7449,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E43</f>
@@ -7467,7 +7458,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E44</f>
@@ -7487,7 +7478,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7498,7 +7489,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7511,7 +7502,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E48</f>
@@ -7520,7 +7511,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E49</f>
@@ -7540,7 +7531,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7551,7 +7542,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7564,7 +7555,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E51</f>
@@ -7573,7 +7564,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E52</f>
@@ -7590,10 +7581,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7642,16 +7633,32 @@
         <v>44084</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D7" s="18">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
+    <row r="8" spans="2:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B8" s="91" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="91"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="20"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7737,7 +7744,7 @@
     </row>
     <row r="11" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="126" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="124" t="s">
         <v>54</v>
@@ -7854,8 +7861,8 @@
   </sheetPr>
   <dimension ref="B2:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E12"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8031,7 +8038,9 @@
         <v>51</v>
       </c>
       <c r="D11" s="106"/>
-      <c r="E11" s="43"/>
+      <c r="E11" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="F11" s="68"/>
       <c r="G11" s="22" t="s">
         <v>67</v>
@@ -8054,7 +8063,9 @@
         <v>65</v>
       </c>
       <c r="D12" s="106"/>
-      <c r="E12" s="43"/>
+      <c r="E12" s="43">
+        <v>2019</v>
+      </c>
       <c r="F12" s="68"/>
       <c r="G12" s="22" t="s">
         <v>66</v>
@@ -8116,7 +8127,7 @@
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="30"/>
       <c r="C15" s="35" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="D15" s="78"/>
       <c r="E15" s="79"/>
@@ -8134,7 +8145,7 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="77"/>
@@ -8171,7 +8182,7 @@
     <row r="18" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="135" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D18" s="89"/>
       <c r="E18" s="86"/>
@@ -8198,10 +8209,10 @@
     <row r="19" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="134" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19" s="150"/>
       <c r="F19" s="94"/>
@@ -8217,17 +8228,17 @@
       </c>
       <c r="N19" s="46"/>
       <c r="O19" s="113" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="P19" s="115"/>
     </row>
     <row r="20" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="90" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" s="90" t="s">
-        <v>77</v>
       </c>
       <c r="E20" s="150">
         <f>1-E19</f>
@@ -8243,7 +8254,7 @@
       <c r="M20" s="88"/>
       <c r="N20" s="46"/>
       <c r="O20" s="113" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="P20" s="115"/>
     </row>
@@ -8270,10 +8281,10 @@
     <row r="22" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="134" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D22" s="106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22" s="150"/>
       <c r="F22" s="94"/>
@@ -8285,17 +8296,17 @@
       <c r="M22" s="88"/>
       <c r="N22" s="46"/>
       <c r="O22" s="113" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="P22" s="115"/>
     </row>
     <row r="23" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
       <c r="C23" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="106" t="s">
         <v>76</v>
-      </c>
-      <c r="D23" s="106" t="s">
-        <v>77</v>
       </c>
       <c r="E23" s="150">
         <f>1-E22</f>
@@ -8311,7 +8322,7 @@
       <c r="M23" s="88"/>
       <c r="N23" s="46"/>
       <c r="O23" s="113" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="P23" s="115"/>
     </row>
@@ -8335,7 +8346,7 @@
     <row r="25" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
       <c r="C25" s="135" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="D25" s="89"/>
       <c r="E25" s="86"/>
@@ -8362,10 +8373,10 @@
     <row r="26" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26" s="134" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" s="150"/>
       <c r="F26" s="94"/>
@@ -8381,17 +8392,17 @@
       </c>
       <c r="N26" s="46"/>
       <c r="O26" s="113" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="P26" s="115"/>
     </row>
     <row r="27" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
       <c r="C27" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="90" t="s">
         <v>76</v>
-      </c>
-      <c r="D27" s="90" t="s">
-        <v>77</v>
       </c>
       <c r="E27" s="150">
         <f>1-E26</f>
@@ -8407,7 +8418,7 @@
       <c r="M27" s="88"/>
       <c r="N27" s="46"/>
       <c r="O27" s="113" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="P27" s="115"/>
     </row>
@@ -8434,10 +8445,10 @@
     <row r="29" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
       <c r="C29" s="134" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D29" s="106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" s="150"/>
       <c r="F29" s="94"/>
@@ -8449,17 +8460,17 @@
       <c r="M29" s="88"/>
       <c r="N29" s="46"/>
       <c r="O29" s="113" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="P29" s="115"/>
     </row>
     <row r="30" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
       <c r="C30" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="106" t="s">
         <v>76</v>
-      </c>
-      <c r="D30" s="106" t="s">
-        <v>77</v>
       </c>
       <c r="E30" s="150">
         <f>1-E29</f>
@@ -8475,7 +8486,7 @@
       <c r="M30" s="88"/>
       <c r="N30" s="46"/>
       <c r="O30" s="113" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="P30" s="115"/>
     </row>
@@ -8499,7 +8510,7 @@
     <row r="32" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
       <c r="C32" s="135" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="D32" s="89"/>
       <c r="E32" s="86"/>
@@ -8526,10 +8537,10 @@
     <row r="33" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
       <c r="C33" s="134" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E33" s="150"/>
       <c r="F33" s="94"/>
@@ -8545,17 +8556,17 @@
       </c>
       <c r="N33" s="46"/>
       <c r="O33" s="113" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="P33" s="115"/>
     </row>
     <row r="34" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
       <c r="C34" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="90" t="s">
         <v>76</v>
-      </c>
-      <c r="D34" s="90" t="s">
-        <v>77</v>
       </c>
       <c r="E34" s="150">
         <f>1-E33</f>
@@ -8571,7 +8582,7 @@
       <c r="M34" s="88"/>
       <c r="N34" s="46"/>
       <c r="O34" s="113" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="P34" s="115"/>
     </row>
@@ -8598,10 +8609,10 @@
     <row r="36" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
       <c r="C36" s="134" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D36" s="106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="150"/>
       <c r="F36" s="94"/>
@@ -8613,17 +8624,17 @@
       <c r="M36" s="88"/>
       <c r="N36" s="46"/>
       <c r="O36" s="113" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="P36" s="115"/>
     </row>
     <row r="37" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
       <c r="C37" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="106" t="s">
         <v>76</v>
-      </c>
-      <c r="D37" s="106" t="s">
-        <v>77</v>
       </c>
       <c r="E37" s="150">
         <f>1-E36</f>
@@ -8639,7 +8650,7 @@
       <c r="M37" s="88"/>
       <c r="N37" s="46"/>
       <c r="O37" s="113" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="P37" s="115"/>
     </row>
@@ -8662,7 +8673,7 @@
     </row>
     <row r="39" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="32" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C39" s="134"/>
       <c r="D39" s="106"/>
@@ -8685,10 +8696,10 @@
     <row r="40" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
       <c r="C40" s="134" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D40" s="90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40" s="150"/>
       <c r="F40" s="94"/>
@@ -8704,17 +8715,17 @@
       </c>
       <c r="N40" s="46"/>
       <c r="O40" s="113" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="P40" s="115"/>
     </row>
     <row r="41" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
       <c r="C41" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="90" t="s">
         <v>76</v>
-      </c>
-      <c r="D41" s="90" t="s">
-        <v>77</v>
       </c>
       <c r="E41" s="150">
         <f>1-E40</f>
@@ -8730,7 +8741,7 @@
       <c r="M41" s="88"/>
       <c r="N41" s="46"/>
       <c r="O41" s="113" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="P41" s="115"/>
     </row>
@@ -8757,10 +8768,10 @@
     <row r="43" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
       <c r="C43" s="134" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D43" s="106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43" s="150"/>
       <c r="F43" s="94"/>
@@ -8772,17 +8783,17 @@
       <c r="M43" s="88"/>
       <c r="N43" s="46"/>
       <c r="O43" s="113" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="P43" s="115"/>
     </row>
     <row r="44" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
       <c r="C44" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="106" t="s">
         <v>76</v>
-      </c>
-      <c r="D44" s="106" t="s">
-        <v>77</v>
       </c>
       <c r="E44" s="150">
         <f>1-E43</f>
@@ -8798,7 +8809,7 @@
       <c r="M44" s="88"/>
       <c r="N44" s="46"/>
       <c r="O44" s="113" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="P44" s="115"/>
     </row>
@@ -8838,7 +8849,7 @@
     </row>
     <row r="47" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="32" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C47" s="134"/>
       <c r="D47" s="106"/>
@@ -8861,10 +8872,10 @@
     <row r="48" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
       <c r="C48" s="134" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D48" s="90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E48" s="150"/>
       <c r="F48" s="94"/>
@@ -8880,17 +8891,17 @@
       </c>
       <c r="N48" s="46"/>
       <c r="O48" s="113" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="P48" s="115"/>
     </row>
     <row r="49" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="32"/>
       <c r="C49" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="90" t="s">
         <v>76</v>
-      </c>
-      <c r="D49" s="90" t="s">
-        <v>77</v>
       </c>
       <c r="E49" s="150">
         <f>1-E48</f>
@@ -8906,7 +8917,7 @@
       <c r="M49" s="88"/>
       <c r="N49" s="46"/>
       <c r="O49" s="113" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="P49" s="115"/>
     </row>
@@ -8933,10 +8944,10 @@
     <row r="51" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="32"/>
       <c r="C51" s="134" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D51" s="106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51" s="150"/>
       <c r="F51" s="94"/>
@@ -8948,17 +8959,17 @@
       <c r="M51" s="88"/>
       <c r="N51" s="46"/>
       <c r="O51" s="113" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="P51" s="115"/>
     </row>
     <row r="52" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="32"/>
       <c r="C52" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="106" t="s">
         <v>76</v>
-      </c>
-      <c r="D52" s="106" t="s">
-        <v>77</v>
       </c>
       <c r="E52" s="150">
         <f>1-E51</f>
@@ -8974,7 +8985,7 @@
       <c r="M52" s="88"/>
       <c r="N52" s="46"/>
       <c r="O52" s="113" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="P52" s="115"/>
     </row>
@@ -9080,62 +9091,62 @@
     <mergeCell ref="B5:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="L10">
-    <cfRule type="cellIs" dxfId="11" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="30" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="29" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L42">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9154,7 +9165,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3073" r:id="rId3" name="import_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!import_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!import_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -9176,7 +9187,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3074" r:id="rId4" name="export_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!export_data_button" altText="export to 'data/…/ouput/molecules’ folder">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!export_data_button" altText="export to 'data/…/ouput/molecules’ folder">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -9198,7 +9209,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="3076" r:id="rId5" name="select_dashboard">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!select_dashboard_values">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!select_dashboard_values">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -9231,7 +9242,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9242,7 +9253,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9255,7 +9266,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E19</f>
@@ -9264,7 +9275,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E20</f>
@@ -9295,7 +9306,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9308,7 +9319,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E22</f>
@@ -9317,7 +9328,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E23</f>
@@ -9336,9 +9347,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9348,7 +9357,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9361,7 +9370,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E26</f>
@@ -9370,7 +9379,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E27</f>
@@ -9389,9 +9398,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9401,7 +9408,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9414,7 +9421,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="B3" s="67">
         <f>Dashboard!E29</f>
@@ -9423,7 +9430,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="67">
         <f>Dashboard!E30</f>

</xml_diff>